<commit_message>
Add tag to packages models
</commit_message>
<xml_diff>
--- a/molgenis-model-registry/src/test/resources/MIAME-ENV.xlsx
+++ b/molgenis-model-registry/src/test/resources/MIAME-ENV.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="69">
   <si>
     <t>name</t>
   </si>
@@ -219,7 +219,16 @@
     <t>Publication</t>
   </si>
   <si>
-    <t>miameenv_home,miameenv_pub1</t>
+    <t>http://www.biosharing.org/bsg-000168</t>
+  </si>
+  <si>
+    <t>Reference</t>
+  </si>
+  <si>
+    <t>miameenv_biosharing</t>
+  </si>
+  <si>
+    <t>miameenv_home,miameenv_pub1,miameenv_biosharing</t>
   </si>
 </sst>
 </file>
@@ -275,7 +284,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="274">
+  <cellStyleXfs count="277">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -548,6 +557,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -556,7 +568,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="271"/>
   </cellXfs>
-  <cellStyles count="274">
+  <cellStyles count="277">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -694,6 +706,9 @@
     <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="273" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="275" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1678,7 +1693,7 @@
         <v>22</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1694,15 +1709,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="47.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1762,6 +1778,26 @@
         <v>58</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated MIAME-ENV for new naming rules
</commit_message>
<xml_diff>
--- a/molgenis-model-registry/src/test/resources/MIAME-ENV.xlsx
+++ b/molgenis-model-registry/src/test/resources/MIAME-ENV.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="29040" windowHeight="16440" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="33000" windowHeight="18140" tabRatio="664"/>
   </bookViews>
   <sheets>
-    <sheet name="entities" sheetId="1" r:id="rId1"/>
-    <sheet name="attributes" sheetId="2" r:id="rId2"/>
-    <sheet name="packages" sheetId="3" r:id="rId3"/>
-    <sheet name="tags" sheetId="4" r:id="rId4"/>
+    <sheet name="entities" sheetId="10" r:id="rId1"/>
+    <sheet name="attributes" sheetId="11" r:id="rId2"/>
+    <sheet name="packages" sheetId="12" r:id="rId3"/>
+    <sheet name="tags" sheetId="13" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="75">
   <si>
     <t>name</t>
   </si>
@@ -93,63 +93,15 @@
     <t>http://mibbi.sourceforge.net/projects/MIAME-Env.shtml</t>
   </si>
   <si>
-    <t>General features</t>
-  </si>
-  <si>
-    <t>Contact Person</t>
-  </si>
-  <si>
-    <t>Key Concepts</t>
-  </si>
-  <si>
     <t>Bibliography</t>
   </si>
   <si>
-    <t>Location of Documents</t>
-  </si>
-  <si>
     <t>Domain</t>
   </si>
   <si>
-    <t>Document Type</t>
-  </si>
-  <si>
-    <t>Group</t>
-  </si>
-  <si>
-    <t>Main Website</t>
-  </si>
-  <si>
-    <t>MI Checklist's Name</t>
-  </si>
-  <si>
-    <t>MI Checklist's Acronym</t>
-  </si>
-  <si>
-    <t>Current Version Designation</t>
-  </si>
-  <si>
-    <t>Release Date for Current Version</t>
-  </si>
-  <si>
-    <t>General Comments</t>
-  </si>
-  <si>
-    <t>Full Name</t>
-  </si>
-  <si>
-    <t>Email Address</t>
-  </si>
-  <si>
     <t>Concept</t>
   </si>
   <si>
-    <t>PubMed Identifier</t>
-  </si>
-  <si>
-    <t>Digital Object Identifier</t>
-  </si>
-  <si>
     <t>URL</t>
   </si>
   <si>
@@ -195,18 +147,18 @@
     <t>relationIRI</t>
   </si>
   <si>
+    <t>miameenv_home</t>
+  </si>
+  <si>
+    <t>Homepage</t>
+  </si>
+  <si>
     <t>system</t>
   </si>
   <si>
     <t>http://molgenis.org/biobankconnect/link</t>
   </si>
   <si>
-    <t>Homepage</t>
-  </si>
-  <si>
-    <t>miameenv_home</t>
-  </si>
-  <si>
     <t>miameenv_pub1</t>
   </si>
   <si>
@@ -216,46 +168,85 @@
     <t>Publication</t>
   </si>
   <si>
+    <t>miameenv_biosharing</t>
+  </si>
+  <si>
+    <t>miameenv_home,miameenv_pub1,miameenv_biosharing</t>
+  </si>
+  <si>
     <t>http://www.biosharing.org/bsg-000168</t>
   </si>
   <si>
     <t>Reference</t>
   </si>
   <si>
-    <t>miameenv_biosharing</t>
-  </si>
-  <si>
-    <t>miameenv_home,miameenv_pub1,miameenv_biosharing</t>
-  </si>
-  <si>
-    <t>[Morrison et al]</t>
-  </si>
-  <si>
-    <t>Biosharing</t>
-  </si>
-  <si>
-    <t>MIAME-Env on Mibbi</t>
-  </si>
-  <si>
     <t>MIAMEENV</t>
   </si>
   <si>
-    <t>MIAMEENV_General features</t>
-  </si>
-  <si>
-    <t>MIAMEENV_Contact Person</t>
-  </si>
-  <si>
-    <t>MIAMEENV_Key Concepts</t>
-  </si>
-  <si>
     <t>MIAMEENV_Concept</t>
   </si>
   <si>
     <t>MIAMEENV_Bibliography</t>
   </si>
   <si>
-    <t>MIAMEENV_Location of Documents</t>
+    <t>MIAMEENV_General_features</t>
+  </si>
+  <si>
+    <t>MIAMEENV_Contact_Person</t>
+  </si>
+  <si>
+    <t>MIAMEENV_Key_Concepts</t>
+  </si>
+  <si>
+    <t>MIAMEENV_Location_of_Documents</t>
+  </si>
+  <si>
+    <t>General_features</t>
+  </si>
+  <si>
+    <t>Contact_Person</t>
+  </si>
+  <si>
+    <t>Key_Concepts</t>
+  </si>
+  <si>
+    <t>Location_of_Documents</t>
+  </si>
+  <si>
+    <t>Digital_Object_Identifier</t>
+  </si>
+  <si>
+    <t>PubMed_Identifier</t>
+  </si>
+  <si>
+    <t>Email_Address</t>
+  </si>
+  <si>
+    <t>Full_Name</t>
+  </si>
+  <si>
+    <t>General_Comments</t>
+  </si>
+  <si>
+    <t>Current_Version_Designation</t>
+  </si>
+  <si>
+    <t>MI_Checklist_s_Acronym</t>
+  </si>
+  <si>
+    <t>MI_Checklist_s_Name</t>
+  </si>
+  <si>
+    <t>Main_Website</t>
+  </si>
+  <si>
+    <t>Document_Type</t>
+  </si>
+  <si>
+    <t>Group_</t>
+  </si>
+  <si>
+    <t>ReleaseDate_Current_Version</t>
   </si>
 </sst>
 </file>
@@ -311,7 +302,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="281">
+  <cellStyleXfs count="274">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -584,13 +575,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -599,7 +583,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="271"/>
   </cellXfs>
-  <cellStyles count="281">
+  <cellStyles count="274">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -737,13 +721,6 @@
     <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="273" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="275" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="277" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="279" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1216,14 +1193,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+    <col min="1" max="1" width="21.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="64.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1243,50 +1219,50 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="B4" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1304,14 +1280,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="7" customWidth="1"/>
     <col min="15" max="15" width="6" customWidth="1"/>
     <col min="16" max="16" width="13" customWidth="1"/>
@@ -1369,10 +1346,10 @@
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="1" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>18</v>
@@ -1399,10 +1376,10 @@
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>18</v>
@@ -1421,10 +1398,10 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>18</v>
@@ -1432,10 +1409,10 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="B5" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>18</v>
@@ -1443,21 +1420,21 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>70</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>18</v>
@@ -1465,10 +1442,10 @@
     </row>
     <row r="8" spans="1:16">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>18</v>
@@ -1476,21 +1453,21 @@
     </row>
     <row r="9" spans="1:16">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>74</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>18</v>
@@ -1498,21 +1475,21 @@
     </row>
     <row r="11" spans="1:16">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="B11" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:16">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>66</v>
       </c>
       <c r="B12" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>18</v>
@@ -1520,13 +1497,13 @@
     </row>
     <row r="13" spans="1:16">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="E13" t="b">
         <v>1</v>
@@ -1537,10 +1514,10 @@
     </row>
     <row r="14" spans="1:16">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>18</v>
@@ -1557,24 +1534,24 @@
     </row>
     <row r="15" spans="1:16">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>18</v>
@@ -1591,10 +1568,10 @@
     </row>
     <row r="17" spans="1:14">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>18</v>
@@ -1602,13 +1579,13 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="E18" t="b">
         <v>1</v>
@@ -1619,32 +1596,32 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:14">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B20" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:14">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>18</v>
@@ -1661,24 +1638,24 @@
     </row>
     <row r="22" spans="1:14">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B22" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:14">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1723,13 +1700,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1748,102 +1725,102 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="47.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="1" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" t="s">
-        <v>70</v>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" t="s">
-        <v>57</v>
+      <c r="A3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" t="s">
-        <v>57</v>
+      <c r="A4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>